<commit_message>
Updated the manual test cases list and added new test cases
</commit_message>
<xml_diff>
--- a/Clean_city_test_cases.xlsx
+++ b/Clean_city_test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLP classes\Software Testing\Week8-career insights\project\wk-6-mah-c-1-glitch-grabbers-team-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282BB4F2-DDC9-440C-B376-7736FE460E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C27828-8D51-4E12-A637-644094680A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{83BF6AED-D74D-4C37-BEFE-C9443779C044}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="223">
   <si>
     <t>Test Scenario Decription</t>
   </si>
@@ -725,6 +725,41 @@
   </si>
   <si>
     <t>The user session should timeout after 45minutes of idle time and should require the user to log in again.</t>
+  </si>
+  <si>
+    <t>TC_BDA_007</t>
+  </si>
+  <si>
+    <t>Verify that a user cannot schedule a pick up for a past date.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the home tab as a user
+2. Fill in the form to schedule a pickup request
+3. on the preferred pickup date section select a date in the past (eg yesterday)
+4. submit the request.</t>
+  </si>
+  <si>
+    <t>The application should prevent users from selecting or submitting a pickup for any past date and should display a validation message.</t>
+  </si>
+  <si>
+    <t>The system accepts the past date and schedules the pickup successfully.</t>
+  </si>
+  <si>
+    <t>TC_EM_004</t>
+  </si>
+  <si>
+    <t>Verify that the application does not accept numerical-only input as a "Full Name".</t>
+  </si>
+  <si>
+    <t>1. Navigate to the waste pickup scheduler.
+2. Enter a numeric-only value in the “Full Name” field (e.g., 12345).
+3. Complete the remaining fields and submit the form</t>
+  </si>
+  <si>
+    <t>The system should validate the “Full Name” field and reject numeric-only inputs, prompting the user to enter a valid name.</t>
+  </si>
+  <si>
+    <t>The application accepts numeric-only names and completes the request successfully.</t>
   </si>
 </sst>
 </file>
@@ -838,7 +873,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -948,7 +983,29 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -960,7 +1017,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1055,6 +1112,57 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1064,59 +1172,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1433,12 +1499,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53DC011-671D-4219-A84E-98227AB9D373}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A9" sqref="A9"/>
-      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
+      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,47 +1524,47 @@
   <sheetData>
     <row r="1" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="21"/>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:10" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="1:10" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
     </row>
     <row r="7" spans="1:10" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
     </row>
     <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1534,10 +1600,10 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="46" t="s">
         <v>84</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1546,7 +1612,7 @@
       <c r="D10" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="36" t="s">
         <v>144</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1566,15 +1632,15 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="44"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="5" t="s">
         <v>104</v>
       </c>
@@ -1592,15 +1658,15 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="44"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="5" t="s">
         <v>105</v>
       </c>
@@ -1618,15 +1684,15 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="44"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="24" t="s">
         <v>105</v>
       </c>
@@ -1656,10 +1722,10 @@
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="46" t="s">
         <v>110</v>
       </c>
       <c r="C15" s="27" t="s">
@@ -1668,7 +1734,7 @@
       <c r="D15" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="37" t="s">
         <v>198</v>
       </c>
       <c r="F15" s="27" t="s">
@@ -1688,15 +1754,15 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="38"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="5" t="s">
         <v>26</v>
       </c>
@@ -1714,15 +1780,15 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="5" t="s">
         <v>195</v>
       </c>
@@ -1740,15 +1806,15 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="45"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="39"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5" t="s">
         <v>114</v>
@@ -1776,10 +1842,10 @@
       <c r="J19" s="16"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="46" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1806,8 +1872,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="44"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="4" t="s">
         <v>32</v>
       </c>
@@ -1832,8 +1898,8 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="44"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="4" t="s">
         <v>33</v>
       </c>
@@ -1858,8 +1924,8 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="44"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -1884,8 +1950,8 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="B24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
@@ -1922,26 +1988,26 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="46" t="s">
         <v>146</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="39" t="s">
         <v>147</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="H26" s="37" t="s">
+      <c r="H26" s="36" t="s">
         <v>49</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -1952,18 +2018,18 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="44"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="47"/>
+      <c r="D27" s="40"/>
       <c r="E27" s="4" t="s">
         <v>116</v>
       </c>
       <c r="F27" s="4"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="38"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="6" t="s">
         <v>50</v>
       </c>
@@ -1972,18 +2038,18 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="44"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="48"/>
+      <c r="D28" s="41"/>
       <c r="E28" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="38"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="6" t="s">
         <v>50</v>
       </c>
@@ -1992,22 +2058,22 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="44"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="36" t="s">
         <v>148</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>118</v>
       </c>
       <c r="F29" s="5"/>
-      <c r="G29" s="49" t="s">
+      <c r="G29" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="H29" s="38"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="6" t="s">
         <v>50</v>
       </c>
@@ -2016,18 +2082,18 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="B30" s="45"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="39"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="5" t="s">
         <v>119</v>
       </c>
       <c r="F30" s="5"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="39"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="38"/>
       <c r="I30" s="6" t="s">
         <v>50</v>
       </c>
@@ -2048,10 +2114,10 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="1:10" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="46" t="s">
         <v>153</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -2080,8 +2146,8 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="4" t="s">
         <v>159</v>
       </c>
@@ -2106,8 +2172,8 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="48"/>
       <c r="C34" s="4" t="s">
         <v>160</v>
       </c>
@@ -2130,7 +2196,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="1" t="s">
         <v>154</v>
       </c>
@@ -2172,237 +2238,237 @@
       <c r="J36" s="16"/>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="37" t="s">
+      <c r="D37" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G37" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="17" t="s">
+      <c r="I37" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="J37" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="5" t="s">
+      <c r="A38" s="50"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="38"/>
-      <c r="E38" s="5" t="s">
+      <c r="D38" s="42"/>
+      <c r="E38" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H38" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="I38" s="18" t="s">
+      <c r="I38" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J38" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="5" t="s">
+      <c r="A39" s="50"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="39"/>
-      <c r="E39" s="5" t="s">
+      <c r="D39" s="42"/>
+      <c r="E39" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G39" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H39" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="I39" s="17" t="s">
+      <c r="I39" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J39" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="5" t="s">
+      <c r="A40" s="50"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="32" t="s">
         <v>139</v>
       </c>
       <c r="F40" s="19">
         <v>45911</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G40" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="H40" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="I40" s="18" t="s">
+      <c r="I40" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J40" s="5" t="s">
+      <c r="J40" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="5" t="s">
+      <c r="A41" s="50"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="32" t="s">
         <v>141</v>
       </c>
       <c r="F41" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="H41" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="I41" s="17" t="s">
+      <c r="I41" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J41" s="5" t="s">
+      <c r="J41" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="5" t="s">
+      <c r="A42" s="50"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="I42" s="17" t="s">
+      <c r="I42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J42" s="32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="31"/>
-    </row>
-    <row r="44" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+    <row r="43" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="51"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="F43" s="19">
+        <v>39609</v>
+      </c>
+      <c r="G43" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="H43" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="31"/>
+    </row>
+    <row r="45" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B45" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F45" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="G45" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H45" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="34"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="I45" s="17" t="s">
         <v>16</v>
@@ -2411,79 +2477,91 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="51"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="9" t="s">
+    <row r="46" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="54"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D47" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E47" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F47" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G47" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="H46" s="9" t="s">
+      <c r="H47" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="I46" s="6" t="s">
+      <c r="I47" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J46" s="9" t="s">
+      <c r="J47" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="I48" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="55"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="E48" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="F48" s="32">
+        <v>12345</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="H48" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J48" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -2495,37 +2573,39 @@
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
     </row>
-    <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>176</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>177</v>
+      </c>
       <c r="G50" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I50" s="18" t="s">
-        <v>27</v>
+        <v>179</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -2537,113 +2617,154 @@
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
     </row>
-    <row r="52" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B52" s="35" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I52" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J52" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="I54" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="52"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="9" t="s">
+    <row r="55" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="33"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D55" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E55" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9" t="s">
+      <c r="F55" s="9"/>
+      <c r="G55" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="H55" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="I53" s="11" t="s">
+      <c r="I55" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J53" s="9" t="s">
+      <c r="J55" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-    </row>
-    <row r="55" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+    <row r="56" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C57" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D57" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5" t="s">
+      <c r="F57" s="5"/>
+      <c r="G57" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H57" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="I55" s="18" t="s">
+      <c r="I57" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="J55" s="5" t="s">
+      <c r="J57" s="5" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="H26:H30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A32:A35"/>
@@ -2660,12 +2781,13 @@
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="G26:G28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>